<commit_message>
Adding requirement.txt files, for python env
</commit_message>
<xml_diff>
--- a/working/kitti-odom-eval/plots/vo_evaluation_results.xlsx
+++ b/working/kitti-odom-eval/plots/vo_evaluation_results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K29"/>
+  <dimension ref="A1:K31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -503,32 +503,32 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>9.369</t>
+          <t>72.994</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>1.655</t>
+          <t>31.386</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>45.319</t>
+          <t>315.888</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>45.319</t>
+          <t>315.888</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>0.228</t>
+          <t>0.573</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>0.178</t>
+          <t>1.408</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
@@ -538,12 +538,12 @@
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>1683.407</t>
+          <t>812.400</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>111.756</t>
+          <t>63.388</t>
         </is>
       </c>
     </row>
@@ -560,32 +560,32 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>9.796</t>
+          <t>106.113</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>1.655</t>
+          <t>31.386</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>50.497</t>
+          <t>644.137</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>50.497</t>
+          <t>644.137</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>0.236</t>
+          <t>2.087</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>0.178</t>
+          <t>1.408</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
@@ -595,12 +595,12 @@
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>1786.254</t>
+          <t>1618.587</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>119.101</t>
+          <t>141.722</t>
         </is>
       </c>
     </row>
@@ -617,32 +617,32 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>9.796</t>
+          <t>106.113</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>1.655</t>
+          <t>31.386</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>28.474</t>
+          <t>47.742</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>28.474</t>
+          <t>47.742</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>0.236</t>
+          <t>2.087</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>0.178</t>
+          <t>1.408</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
@@ -652,12 +652,12 @@
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>1786.254</t>
+          <t>1618.587</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>85.034</t>
+          <t>92.346</t>
         </is>
       </c>
     </row>
@@ -674,32 +674,32 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>10.664</t>
+          <t>105.255</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>1.655</t>
+          <t>31.386</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>37.671</t>
+          <t>47.901</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>37.671</t>
+          <t>47.901</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>0.233</t>
+          <t>2.069</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>0.178</t>
+          <t>1.408</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
@@ -714,49 +714,49 @@
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>104.983</t>
+          <t>94.226</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>_2_opticalFlowVo</t>
+          <t>_1_featureBasedVo</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>scale</t>
+          <t>Direct</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>11.729</t>
+          <t>105.255</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>3.182</t>
+          <t>31.386</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>93.931</t>
+          <t>638.392</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>93.931</t>
+          <t>638.392</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>0.090</t>
+          <t>2.069</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>0.271</t>
+          <t>1.408</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
@@ -766,12 +766,12 @@
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>1571.065</t>
+          <t>1590.000</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>141.485</t>
+          <t>139.322</t>
         </is>
       </c>
     </row>
@@ -783,12 +783,12 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>scale_7dof</t>
+          <t>scale</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>10.608</t>
+          <t>17.049</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -798,17 +798,17 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>94.895</t>
+          <t>98.475</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>94.895</t>
+          <t>98.475</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>0.056</t>
+          <t>0.239</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
@@ -823,12 +823,12 @@
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>1630.725</t>
+          <t>1489.335</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>146.717</t>
+          <t>162.313</t>
         </is>
       </c>
     </row>
@@ -840,12 +840,12 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>7dof</t>
+          <t>scale_7dof</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>10.608</t>
+          <t>15.040</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -855,17 +855,17 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>33.701</t>
+          <t>107.464</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>33.701</t>
+          <t>107.464</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>0.056</t>
+          <t>0.215</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
@@ -880,12 +880,12 @@
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>1630.725</t>
+          <t>1670.377</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>70.008</t>
+          <t>182.212</t>
         </is>
       </c>
     </row>
@@ -897,12 +897,12 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>6dof</t>
+          <t>7dof</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>10.200</t>
+          <t>15.040</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -912,17 +912,17 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>35.210</t>
+          <t>44.922</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>35.210</t>
+          <t>44.922</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>0.027</t>
+          <t>0.215</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
@@ -937,54 +937,54 @@
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>1705.051</t>
+          <t>1670.377</t>
         </is>
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>72.242</t>
+          <t>106.486</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>_3_DF_VO</t>
+          <t>_2_opticalFlowVo</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>scale</t>
+          <t>6dof</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>41.492</t>
+          <t>15.423</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>11.506</t>
+          <t>3.182</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>235.655</t>
+          <t>46.173</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>235.655</t>
+          <t>46.173</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>0.517</t>
+          <t>0.219</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>0.495</t>
+          <t>0.271</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
@@ -994,54 +994,54 @@
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>908.202</t>
+          <t>1590.000</t>
         </is>
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>465.575</t>
+          <t>112.540</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>_3_DF_VO</t>
+          <t>_2_opticalFlowVo</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>scale_7dof</t>
+          <t>Direct</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>43.411</t>
+          <t>15.423</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>11.506</t>
+          <t>3.182</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>236.418</t>
+          <t>101.340</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>236.418</t>
+          <t>101.340</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>0.553</t>
+          <t>0.219</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>0.495</t>
+          <t>0.271</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
@@ -1051,12 +1051,12 @@
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>847.057</t>
+          <t>1590.000</t>
         </is>
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>434.497</t>
+          <t>173.377</t>
         </is>
       </c>
     </row>
@@ -1068,12 +1068,12 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>7dof</t>
+          <t>scale</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>43.411</t>
+          <t>41.492</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -1083,17 +1083,17 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>153.251</t>
+          <t>235.655</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>153.251</t>
+          <t>235.655</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>0.553</t>
+          <t>0.517</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
@@ -1108,12 +1108,12 @@
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>847.057</t>
+          <t>908.202</t>
         </is>
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>270.408</t>
+          <t>465.575</t>
         </is>
       </c>
     </row>
@@ -1125,12 +1125,12 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>6dof</t>
+          <t>scale_7dof</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>28.399</t>
+          <t>43.411</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -1140,17 +1140,17 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>202.170</t>
+          <t>236.418</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>202.170</t>
+          <t>236.418</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>0.234</t>
+          <t>0.553</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
@@ -1165,54 +1165,54 @@
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>1517.896</t>
+          <t>847.057</t>
         </is>
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>443.395</t>
+          <t>434.497</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>_4_DF_VisualOdometry</t>
+          <t>_3_DF_VO</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>scale</t>
+          <t>7dof</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>75.049</t>
+          <t>43.411</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>29.687</t>
+          <t>11.506</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>367.076</t>
+          <t>153.251</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>367.076</t>
+          <t>153.251</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>1.050</t>
+          <t>0.553</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>0.848</t>
+          <t>0.495</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
@@ -1222,54 +1222,54 @@
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>44.369</t>
+          <t>847.057</t>
         </is>
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>14.807</t>
+          <t>270.408</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>_4_DF_VisualOdometry</t>
+          <t>_3_DF_VO</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>scale_7dof</t>
+          <t>6dof</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>107.177</t>
+          <t>28.399</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>29.687</t>
+          <t>11.506</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>536.892</t>
+          <t>202.170</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>536.892</t>
+          <t>202.170</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>1.690</t>
+          <t>0.234</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>0.848</t>
+          <t>0.495</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
@@ -1279,54 +1279,54 @@
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>1093.835</t>
+          <t>1517.896</t>
         </is>
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>310.644</t>
+          <t>443.395</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>_4_DF_VisualOdometry</t>
+          <t>_3_DF_VO</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>7dof</t>
+          <t>Direct</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>107.177</t>
+          <t>28.399</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>29.687</t>
+          <t>11.506</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>88.891</t>
+          <t>302.220</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>88.891</t>
+          <t>302.220</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>1.690</t>
+          <t>0.234</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>0.848</t>
+          <t>0.495</t>
         </is>
       </c>
       <c r="I16" t="inlineStr">
@@ -1336,12 +1336,12 @@
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>1093.835</t>
+          <t>1517.896</t>
         </is>
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>178.426</t>
+          <t>775.494</t>
         </is>
       </c>
     </row>
@@ -1353,12 +1353,12 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>6dof</t>
+          <t>scale</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>100.138</t>
+          <t>75.049</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -1368,17 +1368,17 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>95.649</t>
+          <t>367.076</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>95.649</t>
+          <t>367.076</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>1.580</t>
+          <t>1.050</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
@@ -1393,54 +1393,54 @@
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>908.210</t>
+          <t>44.369</t>
         </is>
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>174.403</t>
+          <t>14.807</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>_5_DPVO_VO</t>
+          <t>_4_DF_VisualOdometry</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>scale</t>
+          <t>scale_7dof</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>23.082</t>
+          <t>107.177</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>0.208</t>
+          <t>29.687</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>177.279</t>
+          <t>536.892</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>177.279</t>
+          <t>536.892</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>0.340</t>
+          <t>1.690</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>0.033</t>
+          <t>0.848</t>
         </is>
       </c>
       <c r="I18" t="inlineStr">
@@ -1450,54 +1450,54 @@
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>1939.773</t>
+          <t>1093.835</t>
         </is>
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>369.351</t>
+          <t>310.644</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>_5_DPVO_VO</t>
+          <t>_4_DF_VisualOdometry</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>scale_7dof</t>
+          <t>7dof</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>20.078</t>
+          <t>107.177</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>0.208</t>
+          <t>29.687</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>194.330</t>
+          <t>88.891</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>194.330</t>
+          <t>88.891</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>0.299</t>
+          <t>1.690</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>0.033</t>
+          <t>0.848</t>
         </is>
       </c>
       <c r="I19" t="inlineStr">
@@ -1507,54 +1507,54 @@
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>1459.933</t>
+          <t>1093.835</t>
         </is>
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>279.431</t>
+          <t>178.426</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>_5_DPVO_VO</t>
+          <t>_4_DF_VisualOdometry</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>7dof</t>
+          <t>6dof</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>20.078</t>
+          <t>100.138</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>0.208</t>
+          <t>29.687</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>83.694</t>
+          <t>95.649</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>83.694</t>
+          <t>95.649</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>0.299</t>
+          <t>1.580</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>0.033</t>
+          <t>0.848</t>
         </is>
       </c>
       <c r="I20" t="inlineStr">
@@ -1564,54 +1564,54 @@
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>1459.933</t>
+          <t>908.210</t>
         </is>
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>110.776</t>
+          <t>174.403</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>_5_DPVO_VO</t>
+          <t>_4_DF_VisualOdometry</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>6dof</t>
+          <t>Direct</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>20.078</t>
+          <t>100.138</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>0.208</t>
+          <t>29.687</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>83.694</t>
+          <t>492.205</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>83.694</t>
+          <t>492.205</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>0.299</t>
+          <t>1.580</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>0.033</t>
+          <t>0.848</t>
         </is>
       </c>
       <c r="I21" t="inlineStr">
@@ -1621,19 +1621,19 @@
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>1459.933</t>
+          <t>908.210</t>
         </is>
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>110.776</t>
+          <t>258.143</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>_6_orb_slam2_mono</t>
+          <t>_5_DPVO_VO</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -1643,32 +1643,32 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>20.389</t>
+          <t>23.082</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>0.606</t>
+          <t>0.208</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>146.557</t>
+          <t>177.279</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>146.557</t>
+          <t>177.279</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>0.289</t>
+          <t>0.340</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>0.183</t>
+          <t>0.033</t>
         </is>
       </c>
       <c r="I22" t="inlineStr">
@@ -1678,19 +1678,19 @@
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>1942.803</t>
+          <t>1939.773</t>
         </is>
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>315.449</t>
+          <t>369.351</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>_6_orb_slam2_mono</t>
+          <t>_5_DPVO_VO</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -1700,32 +1700,32 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>18.325</t>
+          <t>20.078</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>0.606</t>
+          <t>0.208</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>166.037</t>
+          <t>194.330</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>166.037</t>
+          <t>194.330</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>0.269</t>
+          <t>0.299</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>0.183</t>
+          <t>0.033</t>
         </is>
       </c>
       <c r="I23" t="inlineStr">
@@ -1735,19 +1735,19 @@
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>1492.796</t>
+          <t>1459.933</t>
         </is>
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>243.765</t>
+          <t>279.431</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>_6_orb_slam2_mono</t>
+          <t>_5_DPVO_VO</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -1757,32 +1757,32 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>18.325</t>
+          <t>20.078</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>0.606</t>
+          <t>0.208</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>75.250</t>
+          <t>83.694</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>75.250</t>
+          <t>83.694</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>0.269</t>
+          <t>0.299</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>0.183</t>
+          <t>0.033</t>
         </is>
       </c>
       <c r="I24" t="inlineStr">
@@ -1792,19 +1792,19 @@
       </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>1492.796</t>
+          <t>1459.933</t>
         </is>
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>101.136</t>
+          <t>110.776</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>_6_orb_slam2_mono</t>
+          <t>_5_DPVO_VO</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -1814,32 +1814,32 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>69.672</t>
+          <t>20.078</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>0.606</t>
+          <t>0.208</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>208.092</t>
+          <t>83.694</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>208.092</t>
+          <t>83.694</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>0.987</t>
+          <t>0.299</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>0.183</t>
+          <t>0.033</t>
         </is>
       </c>
       <c r="I25" t="inlineStr">
@@ -1849,54 +1849,54 @@
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>135.718</t>
+          <t>1459.933</t>
         </is>
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>248.163</t>
+          <t>110.776</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>_6_orb_slam2_stereo</t>
+          <t>_5_DPVO_VO</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>scale</t>
+          <t>Direct</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>2.558</t>
+          <t>20.078</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>0.475</t>
+          <t>0.208</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>13.243</t>
+          <t>194.330</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>13.243</t>
+          <t>194.330</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>0.035</t>
+          <t>0.299</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>0.048</t>
+          <t>0.033</t>
         </is>
       </c>
       <c r="I26" t="inlineStr">
@@ -1906,54 +1906,54 @@
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>1657.458</t>
+          <t>1459.933</t>
         </is>
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>32.164</t>
+          <t>279.431</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>_6_orb_slam2_stereo</t>
+          <t>_6_orb_slam2_mono</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>scale_7dof</t>
+          <t>scale</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>2.158</t>
+          <t>20.389</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>0.475</t>
+          <t>0.606</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>13.761</t>
+          <t>146.557</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>13.761</t>
+          <t>146.557</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>0.027</t>
+          <t>0.289</t>
         </is>
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>0.048</t>
+          <t>0.183</t>
         </is>
       </c>
       <c r="I27" t="inlineStr">
@@ -1963,54 +1963,54 @@
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>1674.343</t>
+          <t>1942.803</t>
         </is>
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>32.454</t>
+          <t>315.449</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>_6_orb_slam2_stereo</t>
+          <t>_6_orb_slam2_mono</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>7dof</t>
+          <t>scale_7dof</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>2.158</t>
+          <t>18.325</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>0.475</t>
+          <t>0.606</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>8.502</t>
+          <t>166.037</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>8.502</t>
+          <t>166.037</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>0.027</t>
+          <t>0.269</t>
         </is>
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>0.048</t>
+          <t>0.183</t>
         </is>
       </c>
       <c r="I28" t="inlineStr">
@@ -2020,69 +2020,183 @@
       </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t>1674.343</t>
+          <t>1492.796</t>
         </is>
       </c>
       <c r="K28" t="inlineStr">
         <is>
-          <t>16.545</t>
+          <t>243.765</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>_6_orb_slam2_stereo</t>
+          <t>_6_orb_slam2_mono</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
+          <t>7dof</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>18.325</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>0.606</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>75.250</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>75.250</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>0.269</t>
+        </is>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>0.183</t>
+        </is>
+      </c>
+      <c r="I29" t="inlineStr">
+        <is>
+          <t>1705.051</t>
+        </is>
+      </c>
+      <c r="J29" t="inlineStr">
+        <is>
+          <t>1492.796</t>
+        </is>
+      </c>
+      <c r="K29" t="inlineStr">
+        <is>
+          <t>101.136</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>_6_orb_slam2_mono</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
           <t>6dof</t>
         </is>
       </c>
-      <c r="C29" t="inlineStr">
-        <is>
-          <t>2.867</t>
-        </is>
-      </c>
-      <c r="D29" t="inlineStr">
-        <is>
-          <t>0.475</t>
-        </is>
-      </c>
-      <c r="E29" t="inlineStr">
-        <is>
-          <t>12.012</t>
-        </is>
-      </c>
-      <c r="F29" t="inlineStr">
-        <is>
-          <t>12.012</t>
-        </is>
-      </c>
-      <c r="G29" t="inlineStr">
-        <is>
-          <t>0.028</t>
-        </is>
-      </c>
-      <c r="H29" t="inlineStr">
-        <is>
-          <t>0.048</t>
-        </is>
-      </c>
-      <c r="I29" t="inlineStr">
-        <is>
-          <t>1705.051</t>
-        </is>
-      </c>
-      <c r="J29" t="inlineStr">
-        <is>
-          <t>1737.176</t>
-        </is>
-      </c>
-      <c r="K29" t="inlineStr">
-        <is>
-          <t>15.542</t>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>69.672</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>0.606</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>208.092</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>208.092</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>0.987</t>
+        </is>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>0.183</t>
+        </is>
+      </c>
+      <c r="I30" t="inlineStr">
+        <is>
+          <t>1705.051</t>
+        </is>
+      </c>
+      <c r="J30" t="inlineStr">
+        <is>
+          <t>135.718</t>
+        </is>
+      </c>
+      <c r="K30" t="inlineStr">
+        <is>
+          <t>248.163</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>_6_orb_slam2_mono</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Direct</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>69.672</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>0.606</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>345.940</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>345.940</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>0.987</t>
+        </is>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>0.183</t>
+        </is>
+      </c>
+      <c r="I31" t="inlineStr">
+        <is>
+          <t>1705.051</t>
+        </is>
+      </c>
+      <c r="J31" t="inlineStr">
+        <is>
+          <t>135.718</t>
+        </is>
+      </c>
+      <c r="K31" t="inlineStr">
+        <is>
+          <t>28.349</t>
         </is>
       </c>
     </row>

</xml_diff>